<commit_message>
This is the last update for Development and Rtaining Center
</commit_message>
<xml_diff>
--- a/employer.xlsx
+++ b/employer.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7A9305-764C-48CD-A715-E54783C0D127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="18960" windowHeight="11835"/>
+    <workbookView xWindow="11070" yWindow="5820" windowWidth="10995" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
@@ -15,27 +16,73 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>اسم الموظف</t>
+  </si>
+  <si>
+    <t>العنوان الوظيفي</t>
+  </si>
+  <si>
+    <t>الرقم الوظيفي</t>
+  </si>
+  <si>
+    <t>مدة الاجازة</t>
+  </si>
+  <si>
+    <t>ت</t>
+  </si>
+  <si>
+    <t>امبجل كاظم نجم</t>
+  </si>
+  <si>
+    <t>مهندس</t>
+  </si>
+  <si>
+    <t>يوم واحد</t>
+  </si>
+  <si>
+    <t>التأريخ</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,23 +90,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="عادي" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="سمة Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="نسق Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -101,7 +174,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,9 +206,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,6 +258,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -342,25 +451,247 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>811327</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -368,12 +699,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>